<commit_message>
corrections to the uniform commitment order xsd and xml
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Criminal_History_Update_Reporting/artifacts/service_model/information_model/IEPD/documentation/Criminal_History_Update_Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Criminal_History_Update_Reporting/artifacts/service_model/information_model/IEPD/documentation/Criminal_History_Update_Mapping.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeljacobson/git/main/shared/ojb-resources-common/src/main/resources/ssp/Criminal_History_Update_Reporting/artifacts/service_model/information_model/IEPD/documentation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E2390E-B297-E245-A6F5-3711611271C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="3180" windowWidth="30720" windowHeight="16080" tabRatio="563"/>
+    <workbookView xWindow="40960" yWindow="1880" windowWidth="30720" windowHeight="19400" tabRatio="563" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -621,7 +627,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -795,7 +801,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -807,22 +813,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -842,9 +842,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -871,6 +868,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1162,14 +1162,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.6640625" style="3" customWidth="1"/>
@@ -1180,43 +1181,43 @@
     <col min="7" max="7" width="159.5" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="15">
-      <c r="A2" s="14" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="18"/>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="10" customFormat="1">
+    <row r="3" spans="1:7" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1230,14 +1231,14 @@
       <c r="E3" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="4" t="s">
         <v>93</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1">
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -1253,14 +1254,14 @@
       <c r="E4" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="4" t="s">
         <v>94</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="28">
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1270,12 +1271,12 @@
       <c r="C5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="28">
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -1288,12 +1289,12 @@
       <c r="D6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="42">
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1303,14 +1304,14 @@
       <c r="C7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="4" t="s">
         <v>145</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="47.25" customHeight="1">
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>82</v>
       </c>
@@ -1323,9 +1324,9 @@
       <c r="E8" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="47.25" customHeight="1">
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>83</v>
       </c>
@@ -1338,9 +1339,9 @@
       <c r="E9" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="28">
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -1353,12 +1354,12 @@
       <c r="D10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="5" customFormat="1">
+    <row r="11" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
@@ -1371,12 +1372,12 @@
       <c r="D11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1">
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
@@ -1389,12 +1390,12 @@
       <c r="D12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1">
+    <row r="13" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>21</v>
       </c>
@@ -1407,12 +1408,12 @@
       <c r="D13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" ht="42">
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>23</v>
       </c>
@@ -1424,205 +1425,205 @@
         <v>54</v>
       </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" s="7" customFormat="1" ht="28">
-      <c r="A15" s="7" t="s">
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="7" customFormat="1">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="7" customFormat="1">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>76</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" s="7" customFormat="1">
-      <c r="A18" s="7" t="s">
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" s="7" customFormat="1">
-      <c r="A19" s="7" t="s">
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>81</v>
       </c>
       <c r="B19" s="4"/>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" s="7" customFormat="1">
-      <c r="A20" s="7" t="s">
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:7" s="7" customFormat="1">
-      <c r="A21" s="7" t="s">
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" s="7" customFormat="1">
-      <c r="A22" s="7" t="s">
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>90</v>
       </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" s="7" customFormat="1">
-      <c r="A23" s="7" t="s">
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" s="7" customFormat="1">
-      <c r="A24" s="7" t="s">
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" s="7" customFormat="1">
-      <c r="A25" s="7" t="s">
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" s="7" customFormat="1">
-      <c r="A26" s="7" t="s">
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" s="7" customFormat="1">
-      <c r="A27" s="7" t="s">
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:7" s="7" customFormat="1">
-      <c r="A28" s="7" t="s">
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B28" s="4"/>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="F28" s="8"/>
-    </row>
-    <row r="29" spans="1:7" s="7" customFormat="1">
-      <c r="A29" s="7" t="s">
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B29" s="4"/>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:7" s="7" customFormat="1">
-      <c r="A30" s="7" t="s">
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
         <v>92</v>
       </c>
       <c r="B30" s="4"/>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" ht="112">
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" s="5" customFormat="1" ht="128" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>25</v>
       </c>
@@ -1632,17 +1633,17 @@
       <c r="C31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="4" t="s">
         <v>153</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" ht="28">
+    <row r="32" spans="1:7" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>27</v>
       </c>
@@ -1655,120 +1656,120 @@
       <c r="D32" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="4" t="s">
         <v>154</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1">
+    <row r="33" spans="1:7" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1">
+    <row r="34" spans="1:7" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>119</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" ht="28">
+    <row r="35" spans="1:7" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>132</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" ht="28">
+    <row r="36" spans="1:7" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" ht="154">
+    <row r="37" spans="1:7" s="5" customFormat="1" ht="176" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1">
+    <row r="38" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F38" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="5" customFormat="1">
+    <row r="39" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="5" customFormat="1" ht="42">
+    <row r="40" spans="1:7" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F40" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="5" customFormat="1" ht="42">
+    <row r="41" spans="1:7" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F41" s="4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="5" customFormat="1" ht="70" customHeight="1">
+    <row r="42" spans="1:7" s="5" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F42" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="5" customFormat="1" ht="70" customHeight="1">
+    <row r="43" spans="1:7" s="5" customFormat="1" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F43" s="4" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="5" customFormat="1" ht="56.25" customHeight="1">
+    <row r="44" spans="1:7" s="5" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>50</v>
       </c>
@@ -1781,17 +1782,17 @@
       <c r="D44" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E44" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="F44" s="4" t="s">
         <v>95</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="5" customFormat="1" ht="37.5" customHeight="1">
+    <row r="45" spans="1:7" s="5" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>43</v>
       </c>
@@ -1804,12 +1805,12 @@
       <c r="D45" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F45" s="8"/>
+      <c r="F45" s="4"/>
       <c r="G45" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="5" customFormat="1" ht="54" customHeight="1">
+    <row r="46" spans="1:7" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>44</v>
       </c>
@@ -1822,12 +1823,12 @@
       <c r="D46" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="F46" s="8"/>
+      <c r="F46" s="4"/>
       <c r="G46" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="5" customFormat="1">
+    <row r="47" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>48</v>
       </c>
@@ -1840,12 +1841,12 @@
       <c r="D47" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F47" s="8"/>
+      <c r="F47" s="4"/>
       <c r="G47" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="5" customFormat="1" ht="33.75" customHeight="1">
+    <row r="48" spans="1:7" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>49</v>
       </c>
@@ -1858,23 +1859,23 @@
       <c r="D48" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F48" s="8"/>
+      <c r="F48" s="4"/>
       <c r="G48" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="12" customFormat="1" ht="93" customHeight="1">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="17" t="s">
+    <row r="49" spans="1:7" s="10" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E49" s="11"/>
+      <c r="E49" s="9"/>
       <c r="F49" s="4"/>
-      <c r="G49" s="11"/>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="G49" s="9"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
     </row>
   </sheetData>
@@ -1894,12 +1895,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1911,12 +1912,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>